<commit_message>
tweak max column width in mdl.FormatScenModelClass()
</commit_message>
<xml_diff>
--- a/Documentation/Issues List.xlsx
+++ b/Documentation/Issues List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Box Sync\Projects\Excel_Steps\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61EC3E3E-5779-4910-866F-2C7301CBFBFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCB2F0EA-8E48-4EE1-8E82-52DBC6149730}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1073" yWindow="1448" windowWidth="18045" windowHeight="14347" xr2:uid="{2CEEE8FD-B73D-4545-B8A4-5EF8ABD8EF55}"/>
+    <workbookView xWindow="1410" yWindow="1785" windowWidth="33608" windowHeight="14348" xr2:uid="{2CEEE8FD-B73D-4545-B8A4-5EF8ABD8EF55}"/>
   </bookViews>
   <sheets>
     <sheet name="Issues List" sheetId="14" r:id="rId1"/>
@@ -380,7 +380,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -421,7 +421,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Accent1" xfId="2" builtinId="29"/>
@@ -758,7 +757,7 @@
     <col min="5" max="5" width="14.6640625" style="17" customWidth="1"/>
     <col min="6" max="7" width="10.6640625" customWidth="1"/>
     <col min="8" max="8" width="9.6640625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="9.1328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.19921875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="44.59765625" style="10" customWidth="1"/>
     <col min="11" max="11" width="27.1328125" customWidth="1"/>
   </cols>
@@ -853,10 +852,12 @@
         <v>14</v>
       </c>
       <c r="G3" s="14"/>
-      <c r="H3" s="20" t="s">
+      <c r="H3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="11"/>
+      <c r="I3" s="11">
+        <v>45251</v>
+      </c>
       <c r="J3" s="9" t="s">
         <v>56</v>
       </c>
@@ -882,8 +883,10 @@
         <v>14</v>
       </c>
       <c r="G4" s="14"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="11"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="11">
+        <v>45251</v>
+      </c>
       <c r="J4" s="9"/>
       <c r="K4" s="9"/>
     </row>
@@ -905,7 +908,7 @@
       </c>
       <c r="F5" s="14"/>
       <c r="G5" s="14"/>
-      <c r="H5" s="20" t="s">
+      <c r="H5" s="5" t="s">
         <v>12</v>
       </c>
       <c r="I5" s="11"/>
@@ -921,7 +924,7 @@
       <c r="E6" s="14"/>
       <c r="F6" s="14"/>
       <c r="G6" s="14"/>
-      <c r="H6" s="20"/>
+      <c r="H6" s="5"/>
       <c r="I6" s="11"/>
       <c r="J6" s="9"/>
     </row>
@@ -933,7 +936,7 @@
       <c r="E7" s="14"/>
       <c r="F7" s="14"/>
       <c r="G7" s="14"/>
-      <c r="H7" s="20"/>
+      <c r="H7" s="5"/>
       <c r="I7" s="11"/>
       <c r="J7" s="9"/>
     </row>
@@ -945,7 +948,7 @@
       <c r="E8" s="14"/>
       <c r="F8" s="14"/>
       <c r="G8" s="14"/>
-      <c r="H8" s="20"/>
+      <c r="H8" s="5"/>
       <c r="I8" s="14"/>
       <c r="J8" s="9"/>
     </row>
@@ -957,7 +960,7 @@
       <c r="E9" s="14"/>
       <c r="F9" s="14"/>
       <c r="G9" s="14"/>
-      <c r="H9" s="20"/>
+      <c r="H9" s="5"/>
       <c r="I9" s="14"/>
       <c r="J9" s="9"/>
     </row>
@@ -969,7 +972,7 @@
       <c r="E10" s="14"/>
       <c r="F10" s="14"/>
       <c r="G10" s="14"/>
-      <c r="H10" s="20"/>
+      <c r="H10" s="5"/>
       <c r="I10" s="14"/>
       <c r="J10" s="9"/>
     </row>
@@ -981,7 +984,7 @@
       <c r="E11" s="14"/>
       <c r="F11" s="14"/>
       <c r="G11" s="14"/>
-      <c r="H11" s="20"/>
+      <c r="H11" s="5"/>
       <c r="I11" s="14"/>
       <c r="J11" s="9"/>
     </row>
@@ -993,7 +996,7 @@
       <c r="E12" s="14"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14"/>
-      <c r="H12" s="20"/>
+      <c r="H12" s="5"/>
       <c r="I12" s="11"/>
       <c r="J12" s="9"/>
     </row>
@@ -1005,7 +1008,7 @@
       <c r="E13" s="14"/>
       <c r="F13" s="14"/>
       <c r="G13" s="14"/>
-      <c r="H13" s="20"/>
+      <c r="H13" s="5"/>
       <c r="I13" s="11"/>
       <c r="J13" s="9"/>
     </row>
@@ -1607,6 +1610,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100131A7E5D4F77A746956415F045A5C926" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a97d9690b8f402e187ab50ff9e207670">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ed469a80-893b-4d10-afe1-2bca84b0b3fe" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a7a62b2823a30264cd03ac7fbb1e3720" ns2:_="">
     <xsd:import namespace="ed469a80-893b-4d10-afe1-2bca84b0b3fe"/>
@@ -1784,12 +1793,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7F2C587D-DE56-4FAF-86B1-77440C7208D8}">
   <ds:schemaRefs>
@@ -1799,6 +1802,15 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A3EAEBD-DA62-40D5-AE35-B46A548088E2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F58C142-E2E2-49FB-BDB2-1F7C8C370D3D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1814,13 +1826,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A3EAEBD-DA62-40D5-AE35-B46A548088E2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>